<commit_message>
auto:fixing changes in the blood draw appoitnment reminder
</commit_message>
<xml_diff>
--- a/config/forms/app/blood_draw_appointment_reminder.xlsx
+++ b/config/forms/app/blood_draw_appointment_reminder.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="87">
   <si>
     <t>type</t>
   </si>
@@ -204,15 +204,16 @@
     <t>notes_app</t>
   </si>
   <si>
-    <t>**Notes about this appoitment:** ${notes}</t>
+    <t>**Notes about this appointment:** ${notes}</t>
+  </si>
+  <si>
+    <t>select_one soon_reminder</t>
   </si>
   <si>
     <t xml:space="preserve">upcoming </t>
   </si>
   <si>
-    <t xml:space="preserve">**Reminder! Client has an appointment soon.**
- **.** Noted, I will follow-up as needed. Delete this Task 
- **.** Keep this reminder in my Task List
+    <t xml:space="preserve">Reminder! Client has an appointment soon.
 </t>
   </si>
   <si>
@@ -246,6 +247,22 @@
     <t>list_name</t>
   </si>
   <si>
+    <t>soon_reminder</t>
+  </si>
+  <si>
+    <t>noted</t>
+  </si>
+  <si>
+    <t>Noted, I will follow-up as needed. Delete this Task</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep this reminder in my Task List
+</t>
+  </si>
+  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -283,7 +300,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -327,6 +344,11 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -398,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -445,11 +467,17 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -459,13 +487,13 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1954,7 +1982,7 @@
       <c r="B37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="14" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="2"/>
@@ -1982,14 +2010,14 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>55</v>
+      <c r="A38" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1999,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -2024,10 +2052,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="15" t="s">
         <v>68</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2184,7 +2212,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2216,6 +2244,28 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
+    <row r="2">
+      <c r="A2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2232,29 +2282,30 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="27.0"/>
+    <col customWidth="1" min="2" max="2" width="26.88"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="19" t="s">
+      <c r="A1" s="19" t="s">
         <v>76</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -2277,25 +2328,25 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="21" t="str">
+      <c r="C2" s="23" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2023-08-20_16-32</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22" t="s">
-        <v>80</v>
+        <v>2023-09-21_08-56</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24" t="s">
+        <v>86</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>

</xml_diff>